<commit_message>
Add equity dashboard, validation, progress indicator, infeasibility diagnosis, and PDF export
- #001: Equity metrics dashboard with preference distribution histogram and satisfaction distribution chart
- #008: Comprehensive input validation at Review stage (missing prefs, invalid shifts, duplicates, etc.)
- #014: Visual progress indicator during solve (Phase 1/2, progress bar, percentage)
- #015: Infeasibility diagnosis with actionable suggestions when solver fails
- #006: Transparency report in Excel export with algorithm explanation and fairness metrics
- Excel export restructured: Report + ShiftAssignments + VolunteerRosters + Audit sheets
- New PDF export for daily shifts (one page per day, formatted tables)
- Default theme changed to light mode
- Updated input template

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/app/public/ShiftSortingHat_InputTemplate.xlsx
+++ b/app/public/ShiftSortingHat_InputTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
@@ -326,118 +326,118 @@
     <t xml:space="preserve">PreAssignedPoints</t>
   </si>
   <si>
-    <t xml:space="preserve">Volunteer 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volunteer 38</t>
+    <t xml:space="preserve">Sam Vimes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrot Ironfoundersson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angua von Überwald</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheery Littlebottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fred Colon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nobby Nobbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detritus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moist von Lipwig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lord Vetinari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adora Belle Dearheart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William de Worde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otto Chriek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Susan Sto Helit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rincewind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twoflower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Luggage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granny Weatherwax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nanny Ogg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magrat Garlick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiffany Aching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Nac Mac Feegle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cohen the Barbarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonard of Quirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Om</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death of Rats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ridcully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Librarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ponder Stibbons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr Pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr Teatime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Auditors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaspode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cut-Me-Own-Throat Dibbler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Havelock Vetinari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esmerelda Weatherwax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brutha</t>
   </si>
 </sst>
 </file>
@@ -577,8 +577,8 @@
   </sheetPr>
   <dimension ref="A1:G987"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4591,12 +4591,13 @@
   </sheetPr>
   <dimension ref="A1:AZ39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.39"/>
   </cols>
   <sheetData>
@@ -4759,7 +4760,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="0" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="6"/>
@@ -4780,7 +4781,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="0" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="6"/>
@@ -4801,7 +4802,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="0" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="6"/>
@@ -4822,7 +4823,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="0" t="s">
         <v>104</v>
       </c>
       <c r="B5" s="6"/>
@@ -4843,7 +4844,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="0" t="s">
         <v>105</v>
       </c>
       <c r="B6" s="6"/>
@@ -4864,7 +4865,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="0" t="s">
         <v>106</v>
       </c>
       <c r="B7" s="6"/>
@@ -4885,7 +4886,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="0" t="s">
         <v>107</v>
       </c>
       <c r="B8" s="6"/>
@@ -4906,7 +4907,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="0" t="s">
         <v>108</v>
       </c>
       <c r="B9" s="6"/>
@@ -4927,7 +4928,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="0" t="s">
         <v>109</v>
       </c>
       <c r="B10" s="6"/>
@@ -4948,7 +4949,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="0" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="6"/>
@@ -4969,7 +4970,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="0" t="s">
         <v>111</v>
       </c>
       <c r="B12" s="6"/>
@@ -4990,7 +4991,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="0" t="s">
         <v>112</v>
       </c>
       <c r="B13" s="6"/>
@@ -5011,7 +5012,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="0" t="s">
         <v>113</v>
       </c>
       <c r="B14" s="6"/>
@@ -5032,7 +5033,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="0" t="s">
         <v>114</v>
       </c>
       <c r="B15" s="6"/>
@@ -5053,7 +5054,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="0" t="s">
         <v>115</v>
       </c>
       <c r="B16" s="6"/>
@@ -5074,7 +5075,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="0" t="s">
         <v>116</v>
       </c>
       <c r="B17" s="6"/>
@@ -5095,7 +5096,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="0" t="s">
         <v>117</v>
       </c>
       <c r="B18" s="6"/>
@@ -5116,7 +5117,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="0" t="s">
         <v>118</v>
       </c>
       <c r="B19" s="6"/>
@@ -5137,7 +5138,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B20" s="6"/>
@@ -5158,7 +5159,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="0" t="s">
         <v>120</v>
       </c>
       <c r="B21" s="6"/>
@@ -5179,7 +5180,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="0" t="s">
         <v>121</v>
       </c>
       <c r="B22" s="6"/>
@@ -5200,7 +5201,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="0" t="s">
         <v>122</v>
       </c>
       <c r="B23" s="6"/>
@@ -5221,7 +5222,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="0" t="s">
         <v>123</v>
       </c>
       <c r="B24" s="6"/>
@@ -5242,7 +5243,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="0" t="s">
         <v>124</v>
       </c>
       <c r="B25" s="6"/>
@@ -5263,7 +5264,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="0" t="s">
         <v>125</v>
       </c>
       <c r="B26" s="6"/>
@@ -5284,7 +5285,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="0" t="s">
         <v>126</v>
       </c>
       <c r="B27" s="6"/>
@@ -5305,7 +5306,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="0" t="s">
         <v>127</v>
       </c>
       <c r="B28" s="6"/>
@@ -5326,7 +5327,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="0" t="s">
         <v>128</v>
       </c>
       <c r="B29" s="6"/>
@@ -5347,7 +5348,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="0" t="s">
         <v>129</v>
       </c>
       <c r="B30" s="6"/>
@@ -5368,7 +5369,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="0" t="s">
         <v>130</v>
       </c>
       <c r="B31" s="6"/>
@@ -5389,7 +5390,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="0" t="s">
         <v>131</v>
       </c>
       <c r="B32" s="6"/>
@@ -5410,7 +5411,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="0" t="s">
         <v>132</v>
       </c>
       <c r="B33" s="6"/>
@@ -5431,7 +5432,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="0" t="s">
         <v>133</v>
       </c>
       <c r="B34" s="6"/>
@@ -5452,7 +5453,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="0" t="s">
         <v>134</v>
       </c>
       <c r="B35" s="6"/>
@@ -5473,7 +5474,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="0" t="s">
         <v>135</v>
       </c>
       <c r="B36" s="6"/>
@@ -5494,7 +5495,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="0" t="s">
         <v>136</v>
       </c>
       <c r="B37" s="6"/>
@@ -5515,7 +5516,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="0" t="s">
         <v>137</v>
       </c>
       <c r="B38" s="6"/>
@@ -5536,7 +5537,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="0" t="s">
         <v>138</v>
       </c>
       <c r="B39" s="6"/>

</xml_diff>